<commit_message>
debug lib and calibration curves
</commit_message>
<xml_diff>
--- a/lib/APGCMS/APGCMS/lib/lib_urine_20160624.xlsx
+++ b/lib/APGCMS/APGCMS/lib/lib_urine_20160624.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27100" yWindow="4040" windowWidth="25040" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="37040" yWindow="10280" windowWidth="25040" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="lib_urine_20160518.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="lib_urine" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="544">
   <si>
     <t>SeqIndex</t>
   </si>
@@ -246,9 +246,6 @@
     <t>HMDB00357</t>
   </si>
   <si>
-    <t>3-hydroxybutyric acid 2TMS</t>
-  </si>
-  <si>
     <t>41 42 43 44 45 46 47 48 49 51 52 53 54 54 55 56 57 58 59 60 61 62 63 64 66 68 69 70 71 72 73 74 75 76 77 78 79 80 81 83 84 85 86 87 88 89 91 92 93 95 96 97 99 100 101 102 103 104 105 106 107 109 110 111 112 113 115 116 117 118 119 120 121 122 125 127 128 129 130 131 132 133 134 135 136 137 138 141 142 143 144 145 147 148 149 150 151 152 153 155 157 158 159 160 161 162 163 164 165 169 171 171 173 174 175 176 177 178 185 186 187 189 191 192 193 194 194 198 201 203 204 205 206 207 209 215 215 217 218 219 221 221 231 233 234 235 236 237 245 247 247 248 249 250 251 257 261 264 281 293 297 324 342 351 397 420 445 471 480 485 501 512 541 552</t>
   </si>
   <si>
@@ -834,9 +831,6 @@
     <t>HMDB00267</t>
   </si>
   <si>
-    <t xml:space="preserve">Pyroglutamic acid </t>
-  </si>
-  <si>
     <t>Pyroglutamic acid (2TMS)</t>
   </si>
   <si>
@@ -999,9 +993,6 @@
     <t>HMDB00857</t>
   </si>
   <si>
-    <t xml:space="preserve">Pimelic acid </t>
-  </si>
-  <si>
     <t>Pimelic acid (2TMS)</t>
   </si>
   <si>
@@ -1029,12 +1020,6 @@
     <t>HMDB00440</t>
   </si>
   <si>
-    <t>m-hydroxyphenylacetic</t>
-  </si>
-  <si>
-    <t>m-hydroxyphenylacetic 2TMS</t>
-  </si>
-  <si>
     <t>40 41 42 43 44 45 46 47 48 49 50 51 52 53 54 55 56 57 58 59 60 61 62 63 64 65 66 67 68 69 70 71 73 74 75 76 77 78 79 80 81 82 83 85 86 87 89 90 91 92 93 94 95 96 97 99 100 101 102 103 104 105 106 107 108 108 109 110 111 112 113 114 115 116 117 118 119 120 121 122 123 124 125 126 127 128 128 129 130 131 132 133 134 135 136 137 138 139 140 140 142 143 144 145 147 148 149 150 151 152 153 154 155 157 159 161 162 163 164 165 166 167 168 169 170 170 171 172 173 174 175 177 178 179 180 181 182 183 184 185 186 187 188 189 191 192 193 194 195 196 197 203 204 205 206 207 208 209 210 211 212 213 215 217 218 219 220 221 222 223 224 225 226 227 228 229 230 232 233 234 235 236 237 238 239 240 241 243 247 248 249 250 252 253 254 255 256 262 263 264 265 266 267 268 269 275 276 278 279 281 282 283 284 285 289 293 294 294 296 297 298 299 300 301 309 313 319 324 325 341 341 342 355 375 379 380 384 407 434 440 461 516 526 531 553 562 576 586 588</t>
   </si>
   <si>
@@ -1329,9 +1314,6 @@
     <t>HMDB00714</t>
   </si>
   <si>
-    <t xml:space="preserve">Hippuric acid </t>
-  </si>
-  <si>
     <t>Hippuric acid 1TMS</t>
   </si>
   <si>
@@ -1473,12 +1455,6 @@
     <t>HMDB00755</t>
   </si>
   <si>
-    <t>4-Hydroxyphenyllactic acid</t>
-  </si>
-  <si>
-    <t>4-Hydroxyphenyllactic acid 3TMS</t>
-  </si>
-  <si>
     <t>40 41 42 43 44 45 46 47 48 49 50 51 52 53 55 56 57 58 59 60 61 62 63 64 65 66 67 68 69 70 71 73 74 75 76 77 78 79 80 81 82 83 84 85 86 87 88 89 90 91 92 93 94 95 96 97 99 101 102 103 104 105 106 107 108 109 110 111 112 112 113 115 116 117 118 119 120 121 122 123 124 125 126 127 128 129 131 132 133 134 135 136 137 138 139 140 141 142 143 144 145 147 148 149 150 151 152 153 154 155 157 158 159 161 162 163 164 165 166 167 168 169 170 171 172 173 174 175 176 177 179 180 181 182 183 184 184 185 186 187 188 189 190 191 192 193 194 195 196 197 198 199 200 201 202 203 204 205 206 207 208 209 210 211 212 213 213 215 216 217 219 220 221 223 224 225 226 226 227 228 229 230 231 232 233 234 235 236 237 238 239 240 241 242 243 245 246 247 249 250 251 252 253 254 255 256 257 258 259 259 260 261 262 263 265 266 267 268 269 270 271 271 274 274 275 276 277 278 279 280 281 282 283 284 285 286 287 289 289 292 293 294 295 296 297 298 299 300 300 302 303 304 305 308 309 310 311 312 313 315 318 321 321 323 324 325 326 327 329 333 334 336 337 338 339 340 341 342 343 344 344 347 350 351 352 353 355 356 357 358 359 360 361 364 365 366 367 368 369 370 370 371 372 377 380 381 383 384 385 386 387 388 391 391 392 394 395 395 396 397 398 399 400 401 402 404 412 413 415 418 421 423 424 426 429 430 431 433 440 442 443 450 451 454 455 465 471 472 475 480 484 502 503 512 513 517 517 522 525 532 532 534 538 540 563 566 572 581 583 596 599</t>
   </si>
   <si>
@@ -1602,12 +1578,6 @@
     <t>HMDB13678</t>
   </si>
   <si>
-    <t>4-hydroxyhippuric Acid</t>
-  </si>
-  <si>
-    <t>4-hydroxyhippuric Acid 2TMS</t>
-  </si>
-  <si>
     <t>40 41 42 43 44 45 46 47 48 49 50 51 52 53 54 55 56 57 58 59 60 61 62 63 64 65 66 67 68 69 70 71 73 74 75 76 77 78 79 80 81 82 83 84 85 86 87 88 89 90 91 92 93 94 95 96 97 98 99 100 101 102 103 104 105 106 107 108 109 110 111 112 113 114 115 116 117 118 119 120 121 122 123 124 125 126 128 129 130 131 132 133 135 136 137 138 139 140 141 141 142 143 144 145 146 147 148 149 150 151 152 153 154 157 158 159 160 161 162 163 164 165 166 167 168 169 171 172 173 174 176 177 178 179 180 181 182 183 184 185 186 187 188 189 190 191 193 194 195 196 197 198 200 201 201 202 203 204 205 206 207 208 209 210 211 212 214 216 217 218 219 220 221 222 223 224 225 226 227 228 229 230 231 232 234 235 236 237 238 239 240 241 241 244 245 246 248 249 250 251 252 253 254 254 255 258 259 261 262 263 264 265 266 267 268 269 270 271 273 274 274 276 276 277 278 279 280 281 282 283 283 285 285 287 289 290 292 294 295 296 297 298 299 300 305 306 306 307 308 309 310 313 314 321 322 323 324 325 326 327 328 332 338 339 340 341 342 343 344 356 361 383 385 396 397 398 401 403 410 411 466 471 472 529 540 587</t>
   </si>
   <si>
@@ -1639,6 +1609,48 @@
   </si>
   <si>
     <t>remove 1TMS</t>
+  </si>
+  <si>
+    <t>Pyroglutamic acid</t>
+  </si>
+  <si>
+    <t>Pimelic acid</t>
+  </si>
+  <si>
+    <t>5-Hydroxyindoleacetic acid</t>
+  </si>
+  <si>
+    <t>O-Hydroxyphenylacetic acid</t>
+  </si>
+  <si>
+    <t>p-Hydroxybenzoic acid</t>
+  </si>
+  <si>
+    <t>Hippuric acid</t>
+  </si>
+  <si>
+    <t>3-hydroxybutyric acid</t>
+  </si>
+  <si>
+    <t>3-hydroxybutyric acid (2TMS)</t>
+  </si>
+  <si>
+    <t>4-hydroxyhippuric acid</t>
+  </si>
+  <si>
+    <t>4-hydroxyhippuric acid (2TMS)</t>
+  </si>
+  <si>
+    <t>3-hydroxyphenylacetic</t>
+  </si>
+  <si>
+    <t>3-hydroxyphenylacetic (2TMS)</t>
+  </si>
+  <si>
+    <t>Hydroxyphenyllactic acid</t>
+  </si>
+  <si>
+    <t>Hydroxyphenyllactic acid (3TMS)</t>
   </si>
 </sst>
 </file>
@@ -1694,8 +1706,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1707,13 +1729,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2045,8 +2077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117:C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2098,7 +2130,7 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2226,7 +2258,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -2259,7 +2291,7 @@
         <v>34</v>
       </c>
       <c r="N5" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2580,10 +2612,10 @@
         <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>536</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>537</v>
       </c>
       <c r="E14">
         <v>12.69</v>
@@ -2601,16 +2633,16 @@
         <v>233</v>
       </c>
       <c r="J14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" t="s">
         <v>76</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" t="s">
         <v>77</v>
-      </c>
-      <c r="L14" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -2618,13 +2650,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
         <v>79</v>
       </c>
-      <c r="C15" t="s">
-        <v>80</v>
-      </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15">
         <v>12.82</v>
@@ -2639,10 +2671,10 @@
         <v>219</v>
       </c>
       <c r="J15" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" t="s">
         <v>81</v>
-      </c>
-      <c r="K15" t="s">
-        <v>82</v>
       </c>
       <c r="L15" t="s">
         <v>17</v>
@@ -2656,13 +2688,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" t="s">
         <v>83</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>84</v>
-      </c>
-      <c r="D16" t="s">
-        <v>85</v>
       </c>
       <c r="E16">
         <v>13.15</v>
@@ -2677,10 +2709,10 @@
         <v>186</v>
       </c>
       <c r="J16" t="s">
+        <v>85</v>
+      </c>
+      <c r="K16" t="s">
         <v>86</v>
-      </c>
-      <c r="K16" t="s">
-        <v>87</v>
       </c>
       <c r="L16" t="s">
         <v>17</v>
@@ -2694,13 +2726,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" t="s">
         <v>88</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>89</v>
-      </c>
-      <c r="D17" t="s">
-        <v>90</v>
       </c>
       <c r="E17">
         <v>13.25</v>
@@ -2715,10 +2747,10 @@
         <v>189</v>
       </c>
       <c r="J17" t="s">
+        <v>90</v>
+      </c>
+      <c r="K17" t="s">
         <v>91</v>
-      </c>
-      <c r="K17" t="s">
-        <v>92</v>
       </c>
       <c r="L17" t="s">
         <v>17</v>
@@ -2732,13 +2764,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
         <v>93</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>94</v>
-      </c>
-      <c r="D18" t="s">
-        <v>95</v>
       </c>
       <c r="E18">
         <v>13.75</v>
@@ -2753,10 +2785,10 @@
         <v>247</v>
       </c>
       <c r="J18" t="s">
+        <v>95</v>
+      </c>
+      <c r="K18" t="s">
         <v>96</v>
-      </c>
-      <c r="K18" t="s">
-        <v>97</v>
       </c>
       <c r="L18" t="s">
         <v>17</v>
@@ -2770,13 +2802,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" t="s">
         <v>88</v>
       </c>
-      <c r="C19" t="s">
-        <v>89</v>
-      </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19">
         <v>13.86</v>
@@ -2791,10 +2823,10 @@
         <v>200</v>
       </c>
       <c r="J19" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" t="s">
         <v>99</v>
-      </c>
-      <c r="K19" t="s">
-        <v>100</v>
       </c>
       <c r="L19" t="s">
         <v>17</v>
@@ -2808,13 +2840,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
         <v>93</v>
       </c>
-      <c r="C20" t="s">
-        <v>94</v>
-      </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20">
         <v>13.92</v>
@@ -2829,10 +2861,10 @@
         <v>247</v>
       </c>
       <c r="J20" t="s">
+        <v>101</v>
+      </c>
+      <c r="K20" t="s">
         <v>102</v>
-      </c>
-      <c r="K20" t="s">
-        <v>103</v>
       </c>
       <c r="L20" t="s">
         <v>17</v>
@@ -2846,13 +2878,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="s">
         <v>104</v>
       </c>
-      <c r="C21" t="s">
-        <v>105</v>
-      </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E21">
         <v>14.04</v>
@@ -2870,16 +2902,16 @@
         <v>24</v>
       </c>
       <c r="J21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K21" t="s">
         <v>106</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" t="s">
         <v>107</v>
-      </c>
-      <c r="L21" t="s">
-        <v>17</v>
-      </c>
-      <c r="M21" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -2887,13 +2919,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>110</v>
-      </c>
-      <c r="D22" t="s">
-        <v>111</v>
       </c>
       <c r="E22">
         <v>14.29</v>
@@ -2908,16 +2940,16 @@
         <v>218</v>
       </c>
       <c r="J22" t="s">
+        <v>111</v>
+      </c>
+      <c r="K22" t="s">
         <v>112</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
+        <v>17</v>
+      </c>
+      <c r="M22" t="s">
         <v>113</v>
-      </c>
-      <c r="L22" t="s">
-        <v>17</v>
-      </c>
-      <c r="M22" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -2925,13 +2957,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" t="s">
         <v>115</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>116</v>
-      </c>
-      <c r="D23" t="s">
-        <v>117</v>
       </c>
       <c r="E23">
         <v>14.62</v>
@@ -2946,10 +2978,10 @@
         <v>177</v>
       </c>
       <c r="J23" t="s">
+        <v>117</v>
+      </c>
+      <c r="K23" t="s">
         <v>118</v>
-      </c>
-      <c r="K23" t="s">
-        <v>119</v>
       </c>
       <c r="L23" t="s">
         <v>17</v>
@@ -2963,13 +2995,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" t="s">
         <v>120</v>
       </c>
-      <c r="C24" t="s">
-        <v>121</v>
-      </c>
       <c r="D24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E24">
         <v>14.85</v>
@@ -2987,16 +3019,16 @@
         <v>105</v>
       </c>
       <c r="J24" t="s">
+        <v>121</v>
+      </c>
+      <c r="K24" t="s">
         <v>122</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" t="s">
         <v>123</v>
-      </c>
-      <c r="L24" t="s">
-        <v>17</v>
-      </c>
-      <c r="M24" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -3004,13 +3036,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
         <v>125</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>126</v>
-      </c>
-      <c r="D25" t="s">
-        <v>127</v>
       </c>
       <c r="E25">
         <v>14.87</v>
@@ -3025,10 +3057,10 @@
         <v>261</v>
       </c>
       <c r="J25" t="s">
+        <v>127</v>
+      </c>
+      <c r="K25" t="s">
         <v>128</v>
-      </c>
-      <c r="K25" t="s">
-        <v>129</v>
       </c>
       <c r="L25" t="s">
         <v>17</v>
@@ -3042,13 +3074,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" t="s">
         <v>125</v>
       </c>
-      <c r="C26" t="s">
-        <v>126</v>
-      </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E26">
         <v>14.95</v>
@@ -3063,10 +3095,10 @@
         <v>261</v>
       </c>
       <c r="J26" t="s">
+        <v>130</v>
+      </c>
+      <c r="K26" t="s">
         <v>131</v>
-      </c>
-      <c r="K26" t="s">
-        <v>132</v>
       </c>
       <c r="L26" t="s">
         <v>17</v>
@@ -3080,13 +3112,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" t="s">
         <v>133</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>134</v>
-      </c>
-      <c r="D27" t="s">
-        <v>135</v>
       </c>
       <c r="E27">
         <v>15.99</v>
@@ -3101,16 +3133,16 @@
         <v>261</v>
       </c>
       <c r="J27" t="s">
+        <v>135</v>
+      </c>
+      <c r="K27" t="s">
         <v>136</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
+        <v>17</v>
+      </c>
+      <c r="M27" t="s">
         <v>137</v>
-      </c>
-      <c r="L27" t="s">
-        <v>17</v>
-      </c>
-      <c r="M27" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -3118,13 +3150,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" t="s">
         <v>139</v>
       </c>
-      <c r="C28" t="s">
-        <v>140</v>
-      </c>
       <c r="D28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E28">
         <v>16.5</v>
@@ -3139,10 +3171,10 @@
         <v>170</v>
       </c>
       <c r="J28" t="s">
+        <v>140</v>
+      </c>
+      <c r="K28" t="s">
         <v>141</v>
-      </c>
-      <c r="K28" t="s">
-        <v>142</v>
       </c>
       <c r="L28" t="s">
         <v>17</v>
@@ -3156,13 +3188,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" t="s">
         <v>143</v>
       </c>
-      <c r="C29" t="s">
-        <v>144</v>
-      </c>
       <c r="D29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E29">
         <v>16.68</v>
@@ -3180,16 +3212,16 @@
         <v>4</v>
       </c>
       <c r="J29" t="s">
+        <v>144</v>
+      </c>
+      <c r="K29" t="s">
         <v>145</v>
       </c>
-      <c r="K29" t="s">
-        <v>146</v>
-      </c>
       <c r="L29" t="s">
         <v>17</v>
       </c>
       <c r="M29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -3197,13 +3229,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" t="s">
         <v>147</v>
       </c>
-      <c r="C30" t="s">
-        <v>148</v>
-      </c>
       <c r="D30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E30">
         <v>16.77</v>
@@ -3221,16 +3253,16 @@
         <v>5</v>
       </c>
       <c r="J30" t="s">
+        <v>148</v>
+      </c>
+      <c r="K30" t="s">
         <v>149</v>
       </c>
-      <c r="K30" t="s">
-        <v>150</v>
-      </c>
       <c r="L30" t="s">
         <v>17</v>
       </c>
       <c r="M30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -3238,13 +3270,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" t="s">
         <v>151</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>152</v>
-      </c>
-      <c r="D31" t="s">
-        <v>153</v>
       </c>
       <c r="E31">
         <v>17</v>
@@ -3259,10 +3291,10 @@
         <v>217</v>
       </c>
       <c r="J31" t="s">
+        <v>153</v>
+      </c>
+      <c r="K31" t="s">
         <v>154</v>
-      </c>
-      <c r="K31" t="s">
-        <v>155</v>
       </c>
       <c r="L31" t="s">
         <v>17</v>
@@ -3276,13 +3308,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" t="s">
         <v>156</v>
       </c>
-      <c r="C32" t="s">
-        <v>157</v>
-      </c>
       <c r="D32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E32">
         <v>17.27</v>
@@ -3297,10 +3329,10 @@
         <v>189</v>
       </c>
       <c r="J32" t="s">
+        <v>157</v>
+      </c>
+      <c r="K32" t="s">
         <v>158</v>
-      </c>
-      <c r="K32" t="s">
-        <v>159</v>
       </c>
       <c r="L32" t="s">
         <v>17</v>
@@ -3314,13 +3346,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" t="s">
         <v>160</v>
       </c>
-      <c r="C33" t="s">
-        <v>161</v>
-      </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E33">
         <v>17.329999999999998</v>
@@ -3335,10 +3367,10 @@
         <v>255</v>
       </c>
       <c r="J33" t="s">
+        <v>161</v>
+      </c>
+      <c r="K33" t="s">
         <v>162</v>
-      </c>
-      <c r="K33" t="s">
-        <v>163</v>
       </c>
       <c r="L33" t="s">
         <v>17</v>
@@ -3352,13 +3384,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" t="s">
         <v>164</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>165</v>
-      </c>
-      <c r="D34" t="s">
-        <v>166</v>
       </c>
       <c r="E34">
         <v>17.399999999999999</v>
@@ -3373,10 +3405,10 @@
         <v>135</v>
       </c>
       <c r="J34" t="s">
+        <v>166</v>
+      </c>
+      <c r="K34" t="s">
         <v>167</v>
-      </c>
-      <c r="K34" t="s">
-        <v>168</v>
       </c>
       <c r="L34" t="s">
         <v>17</v>
@@ -3390,13 +3422,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" t="s">
         <v>169</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>170</v>
-      </c>
-      <c r="D35" t="s">
-        <v>171</v>
       </c>
       <c r="E35">
         <v>17.54</v>
@@ -3411,16 +3443,16 @@
         <v>133</v>
       </c>
       <c r="J35" t="s">
+        <v>171</v>
+      </c>
+      <c r="K35" t="s">
         <v>172</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
+        <v>17</v>
+      </c>
+      <c r="M35" t="s">
         <v>173</v>
-      </c>
-      <c r="L35" t="s">
-        <v>17</v>
-      </c>
-      <c r="M35" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -3428,13 +3460,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36" t="s">
         <v>175</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>176</v>
-      </c>
-      <c r="D36" t="s">
-        <v>177</v>
       </c>
       <c r="E36">
         <v>17.62</v>
@@ -3449,16 +3481,16 @@
         <v>184</v>
       </c>
       <c r="J36" t="s">
+        <v>177</v>
+      </c>
+      <c r="K36" t="s">
         <v>178</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
+        <v>17</v>
+      </c>
+      <c r="M36" t="s">
         <v>179</v>
-      </c>
-      <c r="L36" t="s">
-        <v>17</v>
-      </c>
-      <c r="M36" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -3466,13 +3498,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>180</v>
+      </c>
+      <c r="C37" t="s">
         <v>181</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>182</v>
-      </c>
-      <c r="D37" t="s">
-        <v>183</v>
       </c>
       <c r="E37">
         <v>17.73</v>
@@ -3490,10 +3522,10 @@
         <v>261</v>
       </c>
       <c r="J37" t="s">
+        <v>183</v>
+      </c>
+      <c r="K37" t="s">
         <v>184</v>
-      </c>
-      <c r="K37" t="s">
-        <v>185</v>
       </c>
       <c r="L37" t="s">
         <v>17</v>
@@ -3507,13 +3539,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>185</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" t="s">
         <v>186</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D38" t="s">
-        <v>187</v>
       </c>
       <c r="E38">
         <v>17.78</v>
@@ -3528,10 +3560,10 @@
         <v>159</v>
       </c>
       <c r="J38" t="s">
+        <v>187</v>
+      </c>
+      <c r="K38" t="s">
         <v>188</v>
-      </c>
-      <c r="K38" t="s">
-        <v>189</v>
       </c>
       <c r="L38" t="s">
         <v>17</v>
@@ -3540,7 +3572,7 @@
         <v>61</v>
       </c>
       <c r="N38" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -3548,13 +3580,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" t="s">
         <v>190</v>
       </c>
-      <c r="C39" t="s">
-        <v>191</v>
-      </c>
       <c r="D39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E39">
         <v>17.850000000000001</v>
@@ -3569,16 +3601,16 @@
         <v>292</v>
       </c>
       <c r="J39" t="s">
+        <v>191</v>
+      </c>
+      <c r="K39" t="s">
         <v>192</v>
       </c>
-      <c r="K39" t="s">
-        <v>193</v>
-      </c>
       <c r="L39" t="s">
         <v>17</v>
       </c>
       <c r="M39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -3586,13 +3618,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" t="s">
         <v>194</v>
       </c>
-      <c r="C40" t="s">
-        <v>195</v>
-      </c>
       <c r="D40" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E40">
         <v>17.88</v>
@@ -3610,10 +3642,10 @@
         <v>187</v>
       </c>
       <c r="J40" t="s">
+        <v>195</v>
+      </c>
+      <c r="K40" t="s">
         <v>196</v>
-      </c>
-      <c r="K40" t="s">
-        <v>197</v>
       </c>
       <c r="L40" t="s">
         <v>17</v>
@@ -3627,13 +3659,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C41" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D41" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="E41">
         <v>17.89</v>
@@ -3648,16 +3680,16 @@
         <v>158</v>
       </c>
       <c r="J41" t="s">
+        <v>195</v>
+      </c>
+      <c r="K41" t="s">
         <v>196</v>
       </c>
-      <c r="K41" t="s">
-        <v>197</v>
-      </c>
       <c r="L41" t="s">
         <v>17</v>
       </c>
       <c r="M41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -3668,10 +3700,10 @@
         <v>29</v>
       </c>
       <c r="C42" t="s">
+        <v>198</v>
+      </c>
+      <c r="D42" t="s">
         <v>199</v>
-      </c>
-      <c r="D42" t="s">
-        <v>200</v>
       </c>
       <c r="E42">
         <v>18.79</v>
@@ -3686,16 +3718,16 @@
         <v>158</v>
       </c>
       <c r="J42" t="s">
+        <v>200</v>
+      </c>
+      <c r="K42" t="s">
         <v>201</v>
       </c>
-      <c r="K42" t="s">
-        <v>202</v>
-      </c>
       <c r="L42" t="s">
         <v>17</v>
       </c>
       <c r="M42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -3703,13 +3735,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>202</v>
+      </c>
+      <c r="C43" t="s">
         <v>203</v>
       </c>
-      <c r="C43" t="s">
-        <v>204</v>
-      </c>
       <c r="D43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E43">
         <v>18.93</v>
@@ -3724,16 +3756,16 @@
         <v>222</v>
       </c>
       <c r="J43" t="s">
+        <v>204</v>
+      </c>
+      <c r="K43" t="s">
         <v>205</v>
       </c>
-      <c r="K43" t="s">
-        <v>206</v>
-      </c>
       <c r="L43" t="s">
         <v>17</v>
       </c>
       <c r="M43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -3741,13 +3773,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>206</v>
+      </c>
+      <c r="C44" t="s">
         <v>207</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>208</v>
-      </c>
-      <c r="D44" t="s">
-        <v>209</v>
       </c>
       <c r="E44">
         <v>19.11</v>
@@ -3762,16 +3794,16 @@
         <v>321</v>
       </c>
       <c r="J44" t="s">
+        <v>209</v>
+      </c>
+      <c r="K44" t="s">
         <v>210</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
+        <v>17</v>
+      </c>
+      <c r="M44" t="s">
         <v>211</v>
-      </c>
-      <c r="L44" t="s">
-        <v>17</v>
-      </c>
-      <c r="M44" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -3779,13 +3811,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>212</v>
+      </c>
+      <c r="C45" t="s">
         <v>213</v>
       </c>
-      <c r="C45" t="s">
-        <v>214</v>
-      </c>
       <c r="D45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E45">
         <v>19.260000000000002</v>
@@ -3800,10 +3832,10 @@
         <v>172</v>
       </c>
       <c r="J45" t="s">
+        <v>214</v>
+      </c>
+      <c r="K45" t="s">
         <v>215</v>
-      </c>
-      <c r="K45" t="s">
-        <v>216</v>
       </c>
       <c r="L45" t="s">
         <v>17</v>
@@ -3817,13 +3849,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>216</v>
+      </c>
+      <c r="C46" t="s">
         <v>217</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>218</v>
-      </c>
-      <c r="D46" t="s">
-        <v>219</v>
       </c>
       <c r="E46">
         <v>19.510000000000002</v>
@@ -3838,10 +3870,10 @@
         <v>186</v>
       </c>
       <c r="J46" t="s">
+        <v>219</v>
+      </c>
+      <c r="K46" t="s">
         <v>220</v>
-      </c>
-      <c r="K46" t="s">
-        <v>221</v>
       </c>
       <c r="L46" t="s">
         <v>17</v>
@@ -3855,13 +3887,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>221</v>
+      </c>
+      <c r="C47" t="s">
         <v>222</v>
       </c>
-      <c r="C47" t="s">
-        <v>223</v>
-      </c>
       <c r="D47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E47">
         <v>19.61</v>
@@ -3876,10 +3908,10 @@
         <v>202</v>
       </c>
       <c r="J47" t="s">
+        <v>223</v>
+      </c>
+      <c r="K47" t="s">
         <v>224</v>
-      </c>
-      <c r="K47" t="s">
-        <v>225</v>
       </c>
       <c r="L47" t="s">
         <v>17</v>
@@ -3893,13 +3925,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>225</v>
+      </c>
+      <c r="C48" t="s">
         <v>226</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>227</v>
-      </c>
-      <c r="D48" t="s">
-        <v>228</v>
       </c>
       <c r="E48">
         <v>19.64</v>
@@ -3914,16 +3946,16 @@
         <v>198</v>
       </c>
       <c r="J48" t="s">
+        <v>228</v>
+      </c>
+      <c r="K48" t="s">
         <v>229</v>
       </c>
-      <c r="K48" t="s">
-        <v>230</v>
-      </c>
       <c r="L48" t="s">
         <v>17</v>
       </c>
       <c r="M48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -3931,13 +3963,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>225</v>
+      </c>
+      <c r="C49" t="s">
         <v>226</v>
       </c>
-      <c r="C49" t="s">
-        <v>227</v>
-      </c>
       <c r="D49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E49">
         <v>19.64</v>
@@ -3952,16 +3984,16 @@
         <v>273</v>
       </c>
       <c r="J49" t="s">
+        <v>228</v>
+      </c>
+      <c r="K49" t="s">
         <v>229</v>
       </c>
-      <c r="K49" t="s">
-        <v>230</v>
-      </c>
       <c r="L49" t="s">
         <v>17</v>
       </c>
       <c r="M49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -3969,13 +4001,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>231</v>
+      </c>
+      <c r="C50" t="s">
         <v>232</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>233</v>
-      </c>
-      <c r="D50" t="s">
-        <v>234</v>
       </c>
       <c r="E50">
         <v>19.760000000000002</v>
@@ -3990,16 +4022,16 @@
         <v>259</v>
       </c>
       <c r="J50" t="s">
+        <v>234</v>
+      </c>
+      <c r="K50" t="s">
         <v>235</v>
       </c>
-      <c r="K50" t="s">
-        <v>236</v>
-      </c>
       <c r="L50" t="s">
         <v>17</v>
       </c>
       <c r="M50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -4007,13 +4039,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>236</v>
+      </c>
+      <c r="C51" t="s">
         <v>237</v>
       </c>
-      <c r="C51" t="s">
-        <v>238</v>
-      </c>
       <c r="D51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E51">
         <v>20.36</v>
@@ -4028,16 +4060,16 @@
         <v>259</v>
       </c>
       <c r="J51" t="s">
+        <v>238</v>
+      </c>
+      <c r="K51" t="s">
         <v>239</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
+        <v>17</v>
+      </c>
+      <c r="M51" t="s">
         <v>240</v>
-      </c>
-      <c r="L51" t="s">
-        <v>17</v>
-      </c>
-      <c r="M51" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -4045,13 +4077,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>241</v>
+      </c>
+      <c r="C52" t="s">
         <v>242</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>243</v>
-      </c>
-      <c r="D52" t="s">
-        <v>244</v>
       </c>
       <c r="E52">
         <v>20.48</v>
@@ -4066,16 +4098,16 @@
         <v>209</v>
       </c>
       <c r="J52" t="s">
+        <v>244</v>
+      </c>
+      <c r="K52" t="s">
         <v>245</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
+        <v>17</v>
+      </c>
+      <c r="M52" t="s">
         <v>246</v>
-      </c>
-      <c r="L52" t="s">
-        <v>17</v>
-      </c>
-      <c r="M52" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -4083,13 +4115,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>247</v>
+      </c>
+      <c r="C53" t="s">
         <v>248</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>249</v>
-      </c>
-      <c r="D53" t="s">
-        <v>250</v>
       </c>
       <c r="E53">
         <v>20.55</v>
@@ -4104,10 +4136,10 @@
         <v>216</v>
       </c>
       <c r="J53" t="s">
+        <v>250</v>
+      </c>
+      <c r="K53" t="s">
         <v>251</v>
-      </c>
-      <c r="K53" t="s">
-        <v>252</v>
       </c>
       <c r="L53" t="s">
         <v>17</v>
@@ -4121,13 +4153,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>252</v>
+      </c>
+      <c r="C54" t="s">
         <v>253</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>254</v>
-      </c>
-      <c r="D54" t="s">
-        <v>255</v>
       </c>
       <c r="E54">
         <v>20.75</v>
@@ -4142,16 +4174,16 @@
         <v>335</v>
       </c>
       <c r="J54" t="s">
+        <v>255</v>
+      </c>
+      <c r="K54" t="s">
         <v>256</v>
       </c>
-      <c r="K54" t="s">
-        <v>257</v>
-      </c>
       <c r="L54" t="s">
         <v>17</v>
       </c>
       <c r="M54" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -4159,13 +4191,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>257</v>
+      </c>
+      <c r="C55" t="s">
         <v>258</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>259</v>
-      </c>
-      <c r="D55" t="s">
-        <v>260</v>
       </c>
       <c r="E55">
         <v>20.98</v>
@@ -4180,10 +4212,10 @@
         <v>275</v>
       </c>
       <c r="J55" t="s">
+        <v>260</v>
+      </c>
+      <c r="K55" t="s">
         <v>261</v>
-      </c>
-      <c r="K55" t="s">
-        <v>262</v>
       </c>
       <c r="L55" t="s">
         <v>17</v>
@@ -4197,13 +4229,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C56" t="s">
+        <v>262</v>
+      </c>
+      <c r="D56" t="s">
         <v>263</v>
-      </c>
-      <c r="D56" t="s">
-        <v>264</v>
       </c>
       <c r="E56">
         <v>21.05</v>
@@ -4218,10 +4250,10 @@
         <v>135</v>
       </c>
       <c r="J56" t="s">
+        <v>264</v>
+      </c>
+      <c r="K56" t="s">
         <v>265</v>
-      </c>
-      <c r="K56" t="s">
-        <v>266</v>
       </c>
       <c r="L56" t="s">
         <v>17</v>
@@ -4235,13 +4267,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>247</v>
+      </c>
+      <c r="C57" t="s">
         <v>248</v>
       </c>
-      <c r="C57" t="s">
-        <v>249</v>
-      </c>
       <c r="D57" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E57">
         <v>21.13</v>
@@ -4256,10 +4288,10 @@
         <v>261</v>
       </c>
       <c r="J57" t="s">
+        <v>267</v>
+      </c>
+      <c r="K57" t="s">
         <v>268</v>
-      </c>
-      <c r="K57" t="s">
-        <v>269</v>
       </c>
       <c r="L57" t="s">
         <v>17</v>
@@ -4273,13 +4305,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>269</v>
+      </c>
+      <c r="C58" t="s">
+        <v>530</v>
+      </c>
+      <c r="D58" t="s">
         <v>270</v>
-      </c>
-      <c r="C58" t="s">
-        <v>271</v>
-      </c>
-      <c r="D58" t="s">
-        <v>272</v>
       </c>
       <c r="E58">
         <v>21.29</v>
@@ -4294,10 +4326,10 @@
         <v>258</v>
       </c>
       <c r="J58" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K58" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L58" t="s">
         <v>17</v>
@@ -4311,13 +4343,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>273</v>
+      </c>
+      <c r="C59" t="s">
+        <v>274</v>
+      </c>
+      <c r="D59" t="s">
         <v>275</v>
-      </c>
-      <c r="C59" t="s">
-        <v>276</v>
-      </c>
-      <c r="D59" t="s">
-        <v>277</v>
       </c>
       <c r="E59">
         <v>21.59</v>
@@ -4332,16 +4364,16 @@
         <v>289</v>
       </c>
       <c r="J59" t="s">
+        <v>276</v>
+      </c>
+      <c r="K59" t="s">
+        <v>277</v>
+      </c>
+      <c r="L59" t="s">
+        <v>17</v>
+      </c>
+      <c r="M59" t="s">
         <v>278</v>
-      </c>
-      <c r="K59" t="s">
-        <v>279</v>
-      </c>
-      <c r="L59" t="s">
-        <v>17</v>
-      </c>
-      <c r="M59" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -4349,13 +4381,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>279</v>
+      </c>
+      <c r="C60" t="s">
+        <v>280</v>
+      </c>
+      <c r="D60" t="s">
         <v>281</v>
-      </c>
-      <c r="C60" t="s">
-        <v>282</v>
-      </c>
-      <c r="D60" t="s">
-        <v>283</v>
       </c>
       <c r="E60">
         <v>21.6</v>
@@ -4370,10 +4402,10 @@
         <v>220</v>
       </c>
       <c r="J60" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K60" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L60" t="s">
         <v>17</v>
@@ -4387,13 +4419,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C61" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D61" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E61">
         <v>21.86</v>
@@ -4408,10 +4440,10 @@
         <v>169</v>
       </c>
       <c r="J61" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K61" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L61" t="s">
         <v>17</v>
@@ -4425,13 +4457,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>288</v>
+      </c>
+      <c r="C62" t="s">
+        <v>289</v>
+      </c>
+      <c r="D62" t="s">
         <v>290</v>
-      </c>
-      <c r="C62" t="s">
-        <v>291</v>
-      </c>
-      <c r="D62" t="s">
-        <v>292</v>
       </c>
       <c r="E62">
         <v>22.22</v>
@@ -4449,10 +4481,10 @@
         <v>229</v>
       </c>
       <c r="J62" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K62" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="L62" t="s">
         <v>17</v>
@@ -4466,13 +4498,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C63" t="s">
-        <v>296</v>
+        <v>533</v>
       </c>
       <c r="D63" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E63">
         <v>22.22</v>
@@ -4487,16 +4519,16 @@
         <v>296</v>
       </c>
       <c r="J63" t="s">
+        <v>295</v>
+      </c>
+      <c r="K63" t="s">
+        <v>296</v>
+      </c>
+      <c r="L63" t="s">
+        <v>17</v>
+      </c>
+      <c r="M63" t="s">
         <v>297</v>
-      </c>
-      <c r="K63" t="s">
-        <v>298</v>
-      </c>
-      <c r="L63" t="s">
-        <v>17</v>
-      </c>
-      <c r="M63" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -4504,13 +4536,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>298</v>
+      </c>
+      <c r="C64" t="s">
+        <v>299</v>
+      </c>
+      <c r="D64" t="s">
         <v>300</v>
-      </c>
-      <c r="C64" t="s">
-        <v>301</v>
-      </c>
-      <c r="D64" t="s">
-        <v>302</v>
       </c>
       <c r="E64">
         <v>22.23</v>
@@ -4525,10 +4557,10 @@
         <v>288</v>
       </c>
       <c r="J64" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K64" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L64" t="s">
         <v>17</v>
@@ -4542,13 +4574,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>303</v>
+      </c>
+      <c r="C65" t="s">
+        <v>304</v>
+      </c>
+      <c r="D65" t="s">
         <v>305</v>
-      </c>
-      <c r="C65" t="s">
-        <v>306</v>
-      </c>
-      <c r="D65" t="s">
-        <v>307</v>
       </c>
       <c r="E65">
         <v>22.49</v>
@@ -4563,16 +4595,16 @@
         <v>349</v>
       </c>
       <c r="J65" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K65" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L65" t="s">
         <v>17</v>
       </c>
       <c r="M65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -4580,13 +4612,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>308</v>
+      </c>
+      <c r="C66" t="s">
+        <v>309</v>
+      </c>
+      <c r="D66" t="s">
         <v>310</v>
-      </c>
-      <c r="C66" t="s">
-        <v>311</v>
-      </c>
-      <c r="D66" t="s">
-        <v>312</v>
       </c>
       <c r="E66">
         <v>22.55</v>
@@ -4601,10 +4633,10 @@
         <v>304</v>
       </c>
       <c r="J66" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K66" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L66" t="s">
         <v>17</v>
@@ -4618,13 +4650,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>313</v>
+      </c>
+      <c r="C67" t="s">
+        <v>314</v>
+      </c>
+      <c r="D67" t="s">
         <v>315</v>
-      </c>
-      <c r="C67" t="s">
-        <v>316</v>
-      </c>
-      <c r="D67" t="s">
-        <v>317</v>
       </c>
       <c r="E67">
         <v>22.56</v>
@@ -4639,10 +4671,10 @@
         <v>295</v>
       </c>
       <c r="J67" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="K67" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L67" t="s">
         <v>17</v>
@@ -4656,13 +4688,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C68" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D68" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E68">
         <v>22.55</v>
@@ -4677,10 +4709,10 @@
         <v>288</v>
       </c>
       <c r="J68" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K68" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="L68" t="s">
         <v>17</v>
@@ -4694,13 +4726,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C69" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D69" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E69">
         <v>22.62</v>
@@ -4715,10 +4747,10 @@
         <v>288</v>
       </c>
       <c r="J69" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K69" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L69" t="s">
         <v>17</v>
@@ -4732,13 +4764,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C70" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D70" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E70">
         <v>22.77</v>
@@ -4753,10 +4785,10 @@
         <v>288</v>
       </c>
       <c r="J70" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K70" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L70" t="s">
         <v>17</v>
@@ -4770,13 +4802,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C71" t="s">
-        <v>326</v>
+        <v>531</v>
       </c>
       <c r="D71" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E71">
         <v>22.88</v>
@@ -4791,10 +4823,10 @@
         <v>289</v>
       </c>
       <c r="J71" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="K71" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="L71" t="s">
         <v>17</v>
@@ -4808,13 +4840,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C72" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D72" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E72">
         <v>22.96</v>
@@ -4829,10 +4861,10 @@
         <v>363</v>
       </c>
       <c r="J72" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K72" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="L72" t="s">
         <v>17</v>
@@ -4846,13 +4878,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C73" t="s">
-        <v>336</v>
+        <v>540</v>
       </c>
       <c r="D73" t="s">
-        <v>337</v>
+        <v>541</v>
       </c>
       <c r="E73">
         <v>23</v>
@@ -4867,10 +4899,10 @@
         <v>296</v>
       </c>
       <c r="J73" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="K73" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="L73" t="s">
         <v>17</v>
@@ -4884,13 +4916,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>241</v>
+      </c>
+      <c r="C74" t="s">
         <v>242</v>
       </c>
-      <c r="C74" t="s">
-        <v>243</v>
-      </c>
       <c r="D74" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="E74">
         <v>23.09</v>
@@ -4905,16 +4937,16 @@
         <v>281</v>
       </c>
       <c r="J74" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="K74" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="L74" t="s">
         <v>17</v>
       </c>
       <c r="M74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:13">
@@ -4922,13 +4954,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C75" t="s">
-        <v>344</v>
+        <v>534</v>
       </c>
       <c r="D75" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E75">
         <v>23.31</v>
@@ -4943,16 +4975,16 @@
         <v>223</v>
       </c>
       <c r="J75" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="K75" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="L75" t="s">
         <v>17</v>
       </c>
       <c r="M75" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="76" spans="1:13">
@@ -4960,13 +4992,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C76" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D76" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E76">
         <v>23.58</v>
@@ -4981,16 +5013,16 @@
         <v>296</v>
       </c>
       <c r="J76" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="K76" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="L76" t="s">
         <v>17</v>
       </c>
       <c r="M76" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" spans="1:13">
@@ -4998,13 +5030,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C77" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D77" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E77">
         <v>23.5</v>
@@ -5019,10 +5051,10 @@
         <v>272</v>
       </c>
       <c r="J77" t="s">
+        <v>95</v>
+      </c>
+      <c r="K77" t="s">
         <v>96</v>
-      </c>
-      <c r="K77" t="s">
-        <v>97</v>
       </c>
       <c r="L77" t="s">
         <v>17</v>
@@ -5036,13 +5068,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C78" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="D78" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E78">
         <v>23.68</v>
@@ -5057,10 +5089,10 @@
         <v>300</v>
       </c>
       <c r="J78" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="K78" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="L78" t="s">
         <v>17</v>
@@ -5074,13 +5106,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C79" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D79" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E79">
         <v>23.85</v>
@@ -5095,16 +5127,16 @@
         <v>226</v>
       </c>
       <c r="J79" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="K79" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="L79" t="s">
         <v>17</v>
       </c>
       <c r="M79" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="80" spans="1:13">
@@ -5112,13 +5144,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C80" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D80" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E80">
         <v>23.83</v>
@@ -5133,10 +5165,10 @@
         <v>219</v>
       </c>
       <c r="J80" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="K80" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L80" t="s">
         <v>17</v>
@@ -5150,13 +5182,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C81" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D81" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E81">
         <v>24.08</v>
@@ -5171,10 +5203,10 @@
         <v>318</v>
       </c>
       <c r="J81" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="K81" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="L81" t="s">
         <v>17</v>
@@ -5188,13 +5220,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C82" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D82" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E82">
         <v>24.29</v>
@@ -5212,10 +5244,10 @@
         <v>363</v>
       </c>
       <c r="J82" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="K82" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="L82" t="s">
         <v>17</v>
@@ -5229,13 +5261,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C83" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D83" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="E83">
         <v>24.65</v>
@@ -5250,10 +5282,10 @@
         <v>303</v>
       </c>
       <c r="J83" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="K83" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="L83" t="s">
         <v>17</v>
@@ -5267,13 +5299,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C84" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D84" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E84">
         <v>25.17</v>
@@ -5288,10 +5320,10 @@
         <v>310</v>
       </c>
       <c r="J84" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="K84" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="L84" t="s">
         <v>17</v>
@@ -5305,13 +5337,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C85" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D85" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E85">
         <v>25.28</v>
@@ -5326,16 +5358,16 @@
         <v>194</v>
       </c>
       <c r="J85" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="K85" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="L85" t="s">
         <v>17</v>
       </c>
       <c r="M85" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:13">
@@ -5343,13 +5375,13 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C86" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D86" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="E86">
         <v>25.63</v>
@@ -5364,10 +5396,10 @@
         <v>254</v>
       </c>
       <c r="J86" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="K86" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="L86" t="s">
         <v>17</v>
@@ -5381,13 +5413,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C87" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="D87" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E87">
         <v>25.7</v>
@@ -5402,16 +5434,16 @@
         <v>375</v>
       </c>
       <c r="J87" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="K87" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="L87" t="s">
         <v>17</v>
       </c>
       <c r="M87" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:13">
@@ -5419,13 +5451,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C88" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D88" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="E88">
         <v>25.83</v>
@@ -5440,10 +5472,10 @@
         <v>312</v>
       </c>
       <c r="J88" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="K88" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="L88" t="s">
         <v>17</v>
@@ -5457,13 +5489,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C89" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D89" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="E89">
         <v>25.84</v>
@@ -5478,16 +5510,16 @@
         <v>218</v>
       </c>
       <c r="J89" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="K89" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="L89" t="s">
         <v>17</v>
       </c>
       <c r="M89" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="90" spans="1:13">
@@ -5495,13 +5527,13 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C90" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D90" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="E90">
         <v>26.01</v>
@@ -5516,16 +5548,16 @@
         <v>326</v>
       </c>
       <c r="J90" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="K90" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="L90" t="s">
         <v>17</v>
       </c>
       <c r="M90" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:13">
@@ -5533,13 +5565,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C91" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="D91" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="E91">
         <v>26.23</v>
@@ -5557,10 +5589,10 @@
         <v>341</v>
       </c>
       <c r="J91" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="K91" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="L91" t="s">
         <v>17</v>
@@ -5574,13 +5606,13 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C92" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D92" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="E92">
         <v>26.39</v>
@@ -5595,16 +5627,16 @@
         <v>201</v>
       </c>
       <c r="J92" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="K92" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="L92" t="s">
         <v>17</v>
       </c>
       <c r="M92" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" spans="1:13">
@@ -5612,13 +5644,13 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C93" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D93" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="E93">
         <v>27.02</v>
@@ -5633,10 +5665,10 @@
         <v>465</v>
       </c>
       <c r="J93" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="K93" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="L93" t="s">
         <v>17</v>
@@ -5650,13 +5682,13 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C94" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D94" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E94">
         <v>27.06</v>
@@ -5671,10 +5703,10 @@
         <v>465</v>
       </c>
       <c r="J94" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="K94" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="L94" t="s">
         <v>17</v>
@@ -5688,13 +5720,13 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="C95" t="s">
-        <v>436</v>
+        <v>535</v>
       </c>
       <c r="D95" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="E95">
         <v>27.2</v>
@@ -5709,16 +5741,16 @@
         <v>206</v>
       </c>
       <c r="J95" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="K95" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="L95" t="s">
         <v>17</v>
       </c>
       <c r="M95" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="96" spans="1:13">
@@ -5726,13 +5758,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C96" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D96" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="E96">
         <v>27.32</v>
@@ -5747,10 +5779,10 @@
         <v>479</v>
       </c>
       <c r="J96" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="K96" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="L96" t="s">
         <v>17</v>
@@ -5764,13 +5796,13 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C97" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D97" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E97">
         <v>27.45</v>
@@ -5785,10 +5817,10 @@
         <v>479</v>
       </c>
       <c r="J97" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="K97" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="L97" t="s">
         <v>17</v>
@@ -5802,13 +5834,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C98" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D98" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="E98">
         <v>27.47</v>
@@ -5823,10 +5855,10 @@
         <v>398</v>
       </c>
       <c r="J98" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="K98" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="L98" t="s">
         <v>17</v>
@@ -5840,13 +5872,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C99" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D99" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="E99">
         <v>27.6</v>
@@ -5861,16 +5893,16 @@
         <v>308</v>
       </c>
       <c r="J99" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="K99" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="L99" t="s">
         <v>17</v>
       </c>
       <c r="M99" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="100" spans="1:13">
@@ -5878,13 +5910,13 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C100" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D100" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="E100">
         <v>27.75</v>
@@ -5899,16 +5931,16 @@
         <v>305</v>
       </c>
       <c r="J100" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="K100" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="L100" t="s">
         <v>17</v>
       </c>
       <c r="M100" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="101" spans="1:13">
@@ -5916,13 +5948,13 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C101" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="D101" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E101">
         <v>27.87</v>
@@ -5937,10 +5969,10 @@
         <v>250</v>
       </c>
       <c r="J101" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="K101" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="L101" t="s">
         <v>17</v>
@@ -5954,13 +5986,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="C102" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D102" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="E102">
         <v>27.96</v>
@@ -5975,10 +6007,10 @@
         <v>215</v>
       </c>
       <c r="J102" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="K102" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="L102" t="s">
         <v>17</v>
@@ -5992,13 +6024,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="C103" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D103" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="E103">
         <v>27.98</v>
@@ -6013,10 +6045,10 @@
         <v>371</v>
       </c>
       <c r="J103" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="K103" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="L103" t="s">
         <v>17</v>
@@ -6030,13 +6062,13 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="C104" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D104" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="E104">
         <v>28.39</v>
@@ -6051,16 +6083,16 @@
         <v>247</v>
       </c>
       <c r="J104" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="K104" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="L104" t="s">
         <v>17</v>
       </c>
       <c r="M104" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="105" spans="1:13">
@@ -6068,13 +6100,13 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="C105" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="D105" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="E105">
         <v>28.27</v>
@@ -6089,10 +6121,10 @@
         <v>252</v>
       </c>
       <c r="J105" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="K105" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="L105" t="s">
         <v>17</v>
@@ -6106,13 +6138,13 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="C106" t="s">
-        <v>484</v>
+        <v>542</v>
       </c>
       <c r="D106" t="s">
-        <v>485</v>
+        <v>543</v>
       </c>
       <c r="E106">
         <v>28.29</v>
@@ -6127,16 +6159,16 @@
         <v>308</v>
       </c>
       <c r="J106" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="K106" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="L106" t="s">
         <v>17</v>
       </c>
       <c r="M106" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="107" spans="1:13">
@@ -6144,13 +6176,13 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="C107" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D107" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="E107">
         <v>29.17</v>
@@ -6165,16 +6197,16 @@
         <v>319</v>
       </c>
       <c r="J107" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="K107" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="L107" t="s">
         <v>17</v>
       </c>
       <c r="M107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="108" spans="1:13">
@@ -6182,13 +6214,13 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="C108" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="D108" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="E108">
         <v>29.71</v>
@@ -6203,16 +6235,16 @@
         <v>264</v>
       </c>
       <c r="J108" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="K108" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="L108" t="s">
         <v>17</v>
       </c>
       <c r="M108" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="109" spans="1:13">
@@ -6220,13 +6252,13 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C109" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="D109" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="E109">
         <v>30.12</v>
@@ -6241,10 +6273,10 @@
         <v>305</v>
       </c>
       <c r="J109" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="K109" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="L109" t="s">
         <v>17</v>
@@ -6258,13 +6290,13 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C110" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="D110" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="E110">
         <v>30.17</v>
@@ -6279,16 +6311,16 @@
         <v>338</v>
       </c>
       <c r="J110" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="K110" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="L110" t="s">
         <v>17</v>
       </c>
       <c r="M110" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="111" spans="1:13">
@@ -6296,13 +6328,13 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="C111" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="D111" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="E111">
         <v>30.79</v>
@@ -6317,16 +6349,16 @@
         <v>231</v>
       </c>
       <c r="J111" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="K111" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="L111" t="s">
         <v>17</v>
       </c>
       <c r="M111" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:13">
@@ -6334,13 +6366,13 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="C112" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="D112" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="E112">
         <v>31.03</v>
@@ -6355,10 +6387,10 @@
         <v>243</v>
       </c>
       <c r="J112" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="K112" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="L112" t="s">
         <v>17</v>
@@ -6372,13 +6404,13 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="C113" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="D113" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="E113">
         <v>31.15</v>
@@ -6396,10 +6428,10 @@
         <v>323</v>
       </c>
       <c r="J113" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="K113" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="L113" t="s">
         <v>17</v>
@@ -6413,13 +6445,13 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="C114" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="D114" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="E114">
         <v>31.82</v>
@@ -6437,10 +6469,10 @@
         <v>308</v>
       </c>
       <c r="J114" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="K114" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="L114" t="s">
         <v>17</v>
@@ -6454,13 +6486,13 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="C115" t="s">
-        <v>523</v>
+        <v>532</v>
       </c>
       <c r="D115" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="E115">
         <v>32.82</v>
@@ -6475,16 +6507,16 @@
         <v>335</v>
       </c>
       <c r="J115" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="K115" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="L115" t="s">
         <v>17</v>
       </c>
       <c r="M115" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="116" spans="1:13">
@@ -6492,13 +6524,13 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C116" t="s">
-        <v>527</v>
+        <v>538</v>
       </c>
       <c r="D116" t="s">
-        <v>528</v>
+        <v>539</v>
       </c>
       <c r="E116">
         <v>33.049999999999997</v>
@@ -6516,10 +6548,10 @@
         <v>339</v>
       </c>
       <c r="J116" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="K116" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="L116" t="s">
         <v>17</v>
@@ -6533,13 +6565,13 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="C117" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="D117" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="E117">
         <v>44.25</v>
@@ -6554,16 +6586,16 @@
         <v>458</v>
       </c>
       <c r="J117" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="K117" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="L117" t="s">
         <v>17</v>
       </c>
       <c r="M117" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>